<commit_message>
update error in file path for saving converted document
</commit_message>
<xml_diff>
--- a/static/downloads/convertedFile.xlsx
+++ b/static/downloads/convertedFile.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,22 +470,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>HYPERLINK("https://www.linkedin.com/in/fernando-segura-224988191","Fernando Segura")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/jack-birdsong-a134883b","jack birdsong")</f>
         <v/>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Englewood</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Biomedical Equipment Technician</t>
+          <t>Journeyman Heating, Ventilation, and Air Conditioning Technician</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Conquest One</t>
+          <t xml:space="preserve">Bruce mechanic </t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -496,22 +496,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>HYPERLINK("https://www.linkedin.com/in/jeffrey-w-291999139","Jeffrey W.")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/logan-robinson-608872212","Logan Robinson")</f>
         <v/>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Littleton</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Maintenance Technician II</t>
+          <t>Plumber</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Norgren</t>
+          <t>TONY V. PLUMBING &amp; HEATING, INC</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -522,22 +522,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f>HYPERLINK("https://www.linkedin.com/in/sam-kiega-ba0961168","Sam Kiega")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/daniel-a23","Daniel A.")</f>
         <v/>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Denver Metropolitan Area</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">plant maintenance mechanic </t>
+          <t>Heavy Mobile Equipment Mechanic</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Molson Coors Beverage Company</t>
+          <t>United States Space Force</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -548,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>HYPERLINK("https://www.linkedin.com/in/weston-roberts-7607481a9","Weston Roberts")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/greg-curran-918068106","Greg curran")</f>
         <v/>
       </c>
       <c r="C5" t="inlineStr">
@@ -558,12 +558,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Journeyman Plumber - Superintendent </t>
+          <t>Maintenance Technician</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Performance Plumbing &amp; Heating Inc.</t>
+          <t>Denver water</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -574,22 +574,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <f>HYPERLINK("https://www.linkedin.com/in/sam-metzger-31a196180","Sam Metzger")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/louie-anglo-jr-b1b492171","Louie Anglo Jr")</f>
         <v/>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Denver Metropolitan Area</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Journeyman Plumber</t>
+          <t>Senior plumber</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>US Engineering Laboratories</t>
+          <t>City and County of Denver</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -600,7 +600,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f>HYPERLINK("https://www.linkedin.com/in/cetan-whitebull-49044516b","Cetan  Whitebull")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/brian-mccoy-91054065","Brian McCoy")</f>
         <v/>
       </c>
       <c r="C7" t="inlineStr">
@@ -610,12 +610,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Maintenance Technician</t>
+          <t>Imaging Service Engineer</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Avenue5 Residential</t>
+          <t>CommonSpirit Health</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -626,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f>HYPERLINK("https://www.linkedin.com/in/joshua-martinez-823a24ab","Joshua Martinez")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/john-eastridge-ii-770864195","John Eastridge II")</f>
         <v/>
       </c>
       <c r="C8" t="inlineStr">
@@ -636,12 +636,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Small Business Owner</t>
+          <t>Biomedical Equipment Technician</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>RENOVO Solutions</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -652,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>HYPERLINK("https://www.linkedin.com/in/trey-tellander-63b29852","Trey Tellander")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/julianmeisner","Julian Meisner IV")</f>
         <v/>
       </c>
       <c r="C9" t="inlineStr">
@@ -662,12 +662,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Field Sevice Technician </t>
+          <t>Senior Maintenance Technician</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Motion</t>
+          <t>Camden Property Trust</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -678,22 +678,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <f>HYPERLINK("https://www.linkedin.com/in/charles-blea-b406b8166","Charles Blea")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/robert-sprague-8a28b0154","Robert Sprague")</f>
         <v/>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Metropolitan Area</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Maintenance Supervisor</t>
+          <t>Plumber</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Aramark</t>
+          <t>Roto-Rooter Plumbing and Drain Service</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -704,22 +704,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <f>HYPERLINK("https://www.linkedin.com/in/daneabernathy","Dane Abernathy")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/bill-howard-043235188","Bill Howard")</f>
         <v/>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Denver Metropolitan Area</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Aircraft Maintenance Technician</t>
+          <t>Residential Plumber</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>United States Air Force</t>
+          <t>Canyon Plumbing</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -730,26 +730,382 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <f>HYPERLINK("https://www.linkedin.com/in/jacque-anderson-b72b58113","Jacque Anderson")</f>
+        <f>HYPERLINK("https://www.linkedin.com/in/kevin-bertram-render-9731b6151","Kevin Bertram-Render")</f>
         <v/>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Denver Metropolitan Area</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Maintenance</t>
+          <t>Apprentice Plumber</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>City of Littleton</t>
+          <t>Bates Mechanical, Inc.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>HYPERLINK("https://www.linkedin.com/in/chris-sing-013946142","Chris Sing")</f>
+        <v/>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Master Plumber</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Applewood Plumbing Heating &amp; Electric</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>HYPERLINK("https://www.linkedin.com/in/andrew-romero-70052415b","Andrew Romero")</f>
+        <v/>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Englewood</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Maintenance Technician</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Meadow Gold Dairies</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>HYPERLINK("https://www.linkedin.com/in/jasonbandykarma","Jason Bandy")</f>
+        <v/>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Plumber</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Searching</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>HYPERLINK("https://www.linkedin.com/in/lue-lor-97a725159","Lue Lor")</f>
+        <v/>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Maintenance Technician</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Medtronic</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f>HYPERLINK("https://www.linkedin.com/in/darvi-olivares-097b39135","Darvi Olivares")</f>
+        <v/>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Littleton</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Maintenance Technician</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>MHCD</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f>HYPERLINK("https://www.linkedin.com/in/alex-montgomery-67448a15b","Alex Montgomery")</f>
+        <v/>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Littleton</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Sales Support Representative</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>AEE Solar</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f>HYPERLINK("https://www.linkedin.com/in/brandon-sweet-1aa262a9","Brandon Sweet")</f>
+        <v/>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Littleton</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Plumber</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Wheatridge Plumbing &amp; Heating</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f>HYPERLINK("https://www.linkedin.com/in/josue-flores-3250051a0","Josue Flores")</f>
+        <v/>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Plumber</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Trautman &amp; Shreve, Inc</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f>HYPERLINK("https://www.linkedin.com/in/connor-brady-575a9189","Connor Brady")</f>
+        <v/>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Plumber</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>AAA Service Plumbing, Heating, and Electric</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f>HYPERLINK("https://www.linkedin.com/in/joseph-calimpong-70574969","Joseph Calimpong")</f>
+        <v/>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Denver Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Carwash Maintenance Tech</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Hi Performance Car Wash</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>HYPERLINK("https://www.linkedin.com/in/tyler-hudziec-b322271a2","Tyler Hudziec")</f>
+        <v/>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Denver Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Heating Air Conditioning Specialist</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Denver Public Library</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f>HYPERLINK("https://www.linkedin.com/in/deon-g-575bb7245","Deon G.")</f>
+        <v/>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f>HYPERLINK("https://www.linkedin.com/in/tommy-carrillo-258b00245","Tommy Carrillo")</f>
+        <v/>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Maintenance Technician</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Property Maintenance &amp; Management Services Ltd.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f>HYPERLINK("https://www.linkedin.com/in/jose-saenz-131a96193","Jose Saenz")</f>
+        <v/>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Denver Metropolitan Area</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Licensed apprentice plumber</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>CHS Plumbing</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>